<commit_message>
Added JM_StoredProcedures - 50% Complete
listOfRequirements - highlighted completed
Created:
JM_Debug / DBGeneration.sql, insertData.sql, JM_StoredProcedures.sql
</commit_message>
<xml_diff>
--- a/BSO Report/list of requirments.xlsx
+++ b/BSO Report/list of requirments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SMOKIN_P5YCHO\Documents\GitHub\SOAM-Sullimar-Academy-of-Music\BSO Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2389827B-79D0-477B-9816-E0602745D4BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71B6E58-47CD-4FAD-8BF8-2C106859C6C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2887" yWindow="-12427" windowWidth="9923" windowHeight="11385" xr2:uid="{1DE2ADC3-FEB6-49A7-9182-740603E967D3}"/>
   </bookViews>
@@ -701,7 +701,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C28"/>
+      <selection activeCell="A32" sqref="A32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,13 +1053,13 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="8" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generate Sales reports for course done
</commit_message>
<xml_diff>
--- a/BSO Report/list of requirments.xlsx
+++ b/BSO Report/list of requirments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SMOKIN_P5YCHO\Documents\GitHub\SOAM-Sullimar-Academy-of-Music\BSO Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/112e8136484fc207/Documents/GitHub/SOAM-Sullimar-Academy-of-Music-Enigma-Crackers/BSO Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71B6E58-47CD-4FAD-8BF8-2C106859C6C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F71B6E58-47CD-4FAD-8BF8-2C106859C6C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{87A59031-0B81-4F26-80D7-96249DDA91B1}"/>
   <bookViews>
-    <workbookView xWindow="2887" yWindow="-12427" windowWidth="9923" windowHeight="11385" xr2:uid="{1DE2ADC3-FEB6-49A7-9182-740603E967D3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10360" xr2:uid="{1DE2ADC3-FEB6-49A7-9182-740603E967D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,26 +324,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -700,18 +704,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877E8C4E-DD60-4376-920E-E969433CA291}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:C32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,462 +726,462 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
+    <row r="24" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6">
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6">
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6">
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6">
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6">
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C43" t="s">

</xml_diff>